<commit_message>
first documentation of model
</commit_message>
<xml_diff>
--- a/data/single-bifurcation.xlsx
+++ b/data/single-bifurcation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bramvanmeurs/stack/EPA/Afstuderen - EPA/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83559230-B024-8B4D-BF52-6BB306AF78F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E4378C-6111-AF40-BA75-1BD2E104625D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1087,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F2">
         <v>1</v>

</xml_diff>